<commit_message>
picture for Marker and Style
</commit_message>
<xml_diff>
--- a/DataFileSamples/Settings.xlsx
+++ b/DataFileSamples/Settings.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{986FB1C4-2451-424A-871A-05510E3EA112}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{53031F10-57D7-0A41-A99D-D10436B7BC98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{FBCACF99-A6B6-294D-9E93-9A56262264D9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{FBCACF99-A6B6-294D-9E93-9A56262264D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Color" sheetId="1" r:id="rId1"/>
     <sheet name="Marker" sheetId="2" r:id="rId2"/>
     <sheet name="Style" sheetId="4" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" iterateCount="200" iterateDelta="9.9999999999999995E-7" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
   <si>
     <t>Code</t>
   </si>
@@ -180,9 +181,6 @@
   </si>
   <si>
     <t>r'$\sqrt{2}$'</t>
-  </si>
-  <si>
-    <t>Any latex expression</t>
   </si>
   <si>
     <t>-</t>
@@ -324,6 +322,10 @@
   </si>
   <si>
     <t>grey</t>
+  </si>
+  <si>
+    <t>latex expression</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -579,17 +581,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2248570-B028-AC49-A3FB-F5B7EDB8BDFF}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1039,7 +1041,7 @@
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1053,47 +1055,47 @@
     </row>
     <row r="27" spans="8:8">
       <c r="H27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="8:8">
       <c r="H28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="8:8">
       <c r="H29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="8:8">
       <c r="H30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="8:8">
       <c r="H31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="8:8">
       <c r="H32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="8:8">
       <c r="H33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="8:8">
       <c r="H34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="8:8">
       <c r="H35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1107,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3AB45C-9F31-974C-9314-27D3D6C6A0B9}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1271,9 +1273,146 @@
         <v>50</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C17" s="16"/>
+    </row>
+    <row r="29" spans="1:3" ht="17" thickBot="1"/>
+    <row r="30" spans="1:3" ht="26" thickBot="1">
+      <c r="A30" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="26">
+      <c r="A31" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="26">
+      <c r="A32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="26">
+      <c r="A33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="26">
+      <c r="A34" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="26">
+      <c r="A35" s="13">
+        <v>8</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="26">
+      <c r="A36" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="26">
+      <c r="A37" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="26">
+      <c r="A38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="26">
+      <c r="A39" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="26">
+      <c r="A40" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="26">
+      <c r="A41" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="26">
+      <c r="A42" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="26">
+      <c r="A43" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="26">
+      <c r="A44" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="26">
+      <c r="A45" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="27" thickBot="1">
+      <c r="A46" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1298,7 +1437,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26" thickBot="1">
       <c r="A1" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>19</v>
@@ -1309,37 +1448,37 @@
     </row>
     <row r="2" spans="1:3" ht="25">
       <c r="A2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>53</v>
       </c>
       <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" ht="25">
       <c r="A3" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3" ht="25">
       <c r="A4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:3" ht="25">
       <c r="A5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>58</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>59</v>
       </c>
       <c r="C5" s="19"/>
     </row>
@@ -1348,16 +1487,16 @@
         <v>44</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" ht="25">
       <c r="A7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>62</v>
       </c>
       <c r="C7" s="20"/>
     </row>
@@ -1390,7 +1529,7 @@
     </row>
     <row r="11" spans="1:3" ht="25">
       <c r="A11" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>37</v>
@@ -1399,7 +1538,7 @@
     </row>
     <row r="12" spans="1:3" ht="25">
       <c r="A12" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>39</v>
@@ -1426,10 +1565,10 @@
     </row>
     <row r="15" spans="1:3" ht="25">
       <c r="A15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>64</v>
       </c>
       <c r="C15" s="19"/>
     </row>
@@ -1456,43 +1595,43 @@
         <v>1</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="21"/>
+        <v>64</v>
+      </c>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3" ht="25">
       <c r="A19" s="18">
         <v>2</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="21"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" ht="25">
       <c r="A20" s="18">
         <v>3</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="21"/>
+        <v>66</v>
+      </c>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:3" ht="25">
       <c r="A21" s="18">
         <v>4</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="21"/>
+        <v>67</v>
+      </c>
+      <c r="C21" s="24"/>
     </row>
     <row r="22" spans="1:3" ht="25">
       <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="19"/>
     </row>
@@ -1501,7 +1640,7 @@
         <v>27</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="19"/>
     </row>
@@ -1516,21 +1655,21 @@
     </row>
     <row r="25" spans="1:3" ht="25">
       <c r="A25" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:3" ht="26" thickBot="1">
+      <c r="A26" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:3" ht="26" thickBot="1">
-      <c r="A26" s="22" t="s">
+      <c r="B26" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1540,4 +1679,17 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC46C480-5F93-4248-9246-C85FE685BFBD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>